<commit_message>
SQL server : CASE statement
</commit_message>
<xml_diff>
--- a/SQL_server_nice_commands.xlsx
+++ b/SQL_server_nice_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAMESH\Desktop\Ramesh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E5857C-69BA-45C5-A377-C46AD30DC5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D2949B-D863-4DC4-AEEA-DA1DA0D22A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{621623E7-096E-4161-B3B5-54D77A5E0276}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>command</t>
   </si>
@@ -60,6 +59,18 @@
   </si>
   <si>
     <t>View All Databases/Tables</t>
+  </si>
+  <si>
+    <t>USE DataBaseName;</t>
+  </si>
+  <si>
+    <t>switch to another DataBase</t>
+  </si>
+  <si>
+    <t>SELECT NEWID();</t>
+  </si>
+  <si>
+    <t>returns a guid (globally unique identifier). Return-type is uniqueidentifier</t>
   </si>
 </sst>
 </file>
@@ -421,16 +432,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56D13AB-7362-4122-8670-A9E064088C65}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="59.77734375" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" customWidth="1"/>
+    <col min="2" max="2" width="60.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -465,6 +476,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>